<commit_message>
added realistic flow and inventory capacity data to the case study
</commit_message>
<xml_diff>
--- a/Python/data/case-study/SC-network/locations.xlsx
+++ b/Python/data/case-study/SC-network/locations.xlsx
@@ -1,24 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="27715"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yongjis/Documents/GitHub/msp_models_for_adaptive_disaster_relief_logistics_planning/Python/data/case-study/SC-network/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/local_ysong3/Documents/GitHub/msp_models_for_adaptive_disaster_relief_logistics_planning/Python/data/case-study/SC-network/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCAC7317-7C28-C548-8D42-EB434D50EA4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16840" yWindow="4840" windowWidth="20720" windowHeight="13280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2260" yWindow="7360" windowWidth="44580" windowHeight="19220"/>
   </bookViews>
   <sheets>
     <sheet name="locations" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -31,9 +33,6 @@
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
     <ext uri="GoogleSheetsCustomDataVersion2">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="1wjxvCNDScdaJDwiUwdUu2NgzKvCvFyhKzUUaZz1Drk="/>
     </ext>
@@ -42,12 +41,36 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
+    <author>Microsoft Office User</author>
     <author/>
   </authors>
   <commentList>
-    <comment ref="D6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="I1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Microsoft Office User:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+calculated by the # of pallets multiplied by the number of PoD kits per pallet -- See Emma's kit calculation
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D6" authorId="1">
       <text>
         <r>
           <rPr>
@@ -160,7 +183,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+    <comment ref="D7" authorId="1">
       <text>
         <r>
           <rPr>
@@ -253,14 +276,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="D8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
+    <comment ref="D8" authorId="1">
       <text>
         <r>
           <rPr>
             <sz val="11"/>
             <color theme="1"/>
             <rFont val="Calibri"/>
-            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>======
@@ -273,14 +295,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="B11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
+    <comment ref="B11" authorId="1">
       <text>
         <r>
           <rPr>
             <sz val="11"/>
             <color theme="1"/>
             <rFont val="Calibri"/>
-            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>Same as largest shelter in each state</t>
@@ -450,8 +471,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -476,6 +497,17 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="81"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color indexed="81"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -787,11 +819,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M941"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="O40" sqref="O40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -886,7 +918,10 @@
         <v>34.193145299999998</v>
       </c>
       <c r="H3" s="1"/>
-      <c r="I3" s="12"/>
+      <c r="I3" s="12">
+        <f>4608*50</f>
+        <v>230400</v>
+      </c>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
@@ -913,7 +948,10 @@
         <v>33.614168800000002</v>
       </c>
       <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
+      <c r="I4" s="1">
+        <f>9600*50</f>
+        <v>480000</v>
+      </c>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
@@ -940,7 +978,10 @@
         <v>32.865635400000002</v>
       </c>
       <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
+      <c r="I5" s="1">
+        <f>2400*50</f>
+        <v>120000</v>
+      </c>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
@@ -967,7 +1008,10 @@
         <v>33.230486200000001</v>
       </c>
       <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
+      <c r="I6" s="1">
+        <f>1920*50</f>
+        <v>96000</v>
+      </c>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
@@ -994,7 +1038,10 @@
         <v>32.804634</v>
       </c>
       <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
+      <c r="I7" s="1">
+        <f>3000*50</f>
+        <v>150000</v>
+      </c>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
@@ -1021,7 +1068,10 @@
         <v>33.904211199999999</v>
       </c>
       <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
+      <c r="I8" s="1">
+        <f>2400*50</f>
+        <v>120000</v>
+      </c>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
@@ -1048,7 +1098,10 @@
         <v>34.763020599999997</v>
       </c>
       <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
+      <c r="I9" s="1">
+        <f>14208*50</f>
+        <v>710400</v>
+      </c>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
@@ -1075,7 +1128,10 @@
         <v>34.403608200000001</v>
       </c>
       <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
+      <c r="I10" s="1">
+        <f>1000*50</f>
+        <v>50000</v>
+      </c>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>

</xml_diff>